<commit_message>
Add IPC quantity 13
</commit_message>
<xml_diff>
--- a/progress/data/Structid.xlsx
+++ b/progress/data/Structid.xlsx
@@ -1972,7 +1972,7 @@
   <dimension ref="A1:D357"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J339" sqref="J339"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6991,15 +6991,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.88671875" style="2" customWidth="1"/>
     <col min="3" max="3" width="40.44140625" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -7020,7 +7020,7 @@
       <c r="B2" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>409</v>
       </c>
       <c r="D2" s="2">
@@ -7034,7 +7034,7 @@
       <c r="B3" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>411</v>
       </c>
       <c r="D3" s="2">
@@ -7048,7 +7048,7 @@
       <c r="B4" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>413</v>
       </c>
       <c r="D4" s="2">
@@ -7062,7 +7062,7 @@
       <c r="B5" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>415</v>
       </c>
       <c r="D5" s="2">
@@ -7076,7 +7076,7 @@
       <c r="B6" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>417</v>
       </c>
       <c r="D6" s="2">
@@ -7090,7 +7090,7 @@
       <c r="B7" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D7" s="2">
@@ -7104,7 +7104,7 @@
       <c r="B8" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>421</v>
       </c>
       <c r="D8" s="2">
@@ -7118,7 +7118,7 @@
       <c r="B9" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>422</v>
       </c>
       <c r="D9" s="2">
@@ -7132,7 +7132,7 @@
       <c r="B10" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>424</v>
       </c>
       <c r="D10" s="2">
@@ -7146,7 +7146,7 @@
       <c r="B11" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>426</v>
       </c>
       <c r="D11" s="2">
@@ -7160,7 +7160,7 @@
       <c r="B12" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>428</v>
       </c>
       <c r="D12" s="2">
@@ -7174,7 +7174,7 @@
       <c r="B13" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D13" s="2">
@@ -7188,7 +7188,7 @@
       <c r="B14" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>432</v>
       </c>
       <c r="D14" s="2">
@@ -7202,7 +7202,7 @@
       <c r="B15" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>433</v>
       </c>
       <c r="D15" s="2">
@@ -7216,7 +7216,7 @@
       <c r="B16" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>435</v>
       </c>
       <c r="D16" s="2">
@@ -7230,7 +7230,7 @@
       <c r="B17" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>437</v>
       </c>
       <c r="D17" s="2">
@@ -7244,7 +7244,7 @@
       <c r="B18" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>439</v>
       </c>
       <c r="D18" s="2">
@@ -7258,7 +7258,7 @@
       <c r="B19" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>441</v>
       </c>
       <c r="D19" s="2">
@@ -7272,7 +7272,7 @@
       <c r="B20" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>443</v>
       </c>
       <c r="D20" s="2">
@@ -7286,7 +7286,7 @@
       <c r="B21" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>445</v>
       </c>
       <c r="D21" s="2">
@@ -7300,7 +7300,7 @@
       <c r="B22" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>447</v>
       </c>
       <c r="D22" s="2">
@@ -7314,7 +7314,7 @@
       <c r="B23" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>449</v>
       </c>
       <c r="D23" s="2">
@@ -7328,7 +7328,7 @@
       <c r="B24" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>451</v>
       </c>
       <c r="D24" s="2">
@@ -7342,7 +7342,7 @@
       <c r="B25" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>453</v>
       </c>
       <c r="D25" s="2">
@@ -7356,7 +7356,7 @@
       <c r="B26" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>455</v>
       </c>
       <c r="D26" s="2">
@@ -7370,7 +7370,7 @@
       <c r="B27" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>457</v>
       </c>
       <c r="D27" s="2">
@@ -7384,7 +7384,7 @@
       <c r="B28" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>459</v>
       </c>
       <c r="D28" s="2">
@@ -7398,7 +7398,7 @@
       <c r="B29" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>461</v>
       </c>
       <c r="D29" s="2">
@@ -7412,7 +7412,7 @@
       <c r="B30" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>463</v>
       </c>
       <c r="D30" s="2">
@@ -7426,7 +7426,7 @@
       <c r="B31" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>465</v>
       </c>
       <c r="D31" s="2">
@@ -7440,7 +7440,7 @@
       <c r="B32" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>467</v>
       </c>
       <c r="D32" s="2">
@@ -7454,7 +7454,7 @@
       <c r="B33" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>469</v>
       </c>
       <c r="D33" s="2">
@@ -7468,7 +7468,7 @@
       <c r="B34" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>471</v>
       </c>
       <c r="D34" s="2">
@@ -7482,7 +7482,7 @@
       <c r="B35" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>473</v>
       </c>
       <c r="D35" s="2">
@@ -7496,7 +7496,7 @@
       <c r="B36" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>475</v>
       </c>
       <c r="D36" s="2">
@@ -7510,7 +7510,7 @@
       <c r="B37" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>477</v>
       </c>
       <c r="D37" s="2">
@@ -7524,7 +7524,7 @@
       <c r="B38" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>479</v>
       </c>
       <c r="D38" s="2">
@@ -7538,7 +7538,7 @@
       <c r="B39" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>481</v>
       </c>
       <c r="D39" s="2">
@@ -7552,7 +7552,7 @@
       <c r="B40" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>483</v>
       </c>
       <c r="D40" s="2">
@@ -7566,7 +7566,7 @@
       <c r="B41" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>485</v>
       </c>
       <c r="D41" s="2">
@@ -7580,7 +7580,7 @@
       <c r="B42" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>487</v>
       </c>
       <c r="D42" s="2">
@@ -7594,7 +7594,7 @@
       <c r="B43" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>489</v>
       </c>
       <c r="D43" s="2">
@@ -7608,7 +7608,7 @@
       <c r="B44" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>491</v>
       </c>
       <c r="D44" s="2">
@@ -7622,7 +7622,7 @@
       <c r="B45" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>493</v>
       </c>
       <c r="D45" s="2">
@@ -7636,7 +7636,7 @@
       <c r="B46" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>495</v>
       </c>
       <c r="D46" s="2">
@@ -7650,7 +7650,7 @@
       <c r="B47" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>497</v>
       </c>
       <c r="D47" s="2">
@@ -7664,7 +7664,7 @@
       <c r="B48" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>499</v>
       </c>
       <c r="D48" s="2">
@@ -7678,7 +7678,7 @@
       <c r="B49" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>459</v>
       </c>
       <c r="D49" s="2">
@@ -7692,7 +7692,7 @@
       <c r="B50" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>502</v>
       </c>
       <c r="D50" s="2">
@@ -7706,7 +7706,7 @@
       <c r="B51" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>504</v>
       </c>
       <c r="D51" s="2">
@@ -7720,7 +7720,7 @@
       <c r="B52" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>506</v>
       </c>
       <c r="D52" s="2">
@@ -7734,7 +7734,7 @@
       <c r="B53" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>508</v>
       </c>
       <c r="D53" s="2">
@@ -7748,7 +7748,7 @@
       <c r="B54" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>510</v>
       </c>
       <c r="D54" s="2">
@@ -7762,7 +7762,7 @@
       <c r="B55" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>512</v>
       </c>
       <c r="D55" s="2">
@@ -7776,7 +7776,7 @@
       <c r="B56" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>514</v>
       </c>
       <c r="D56" s="2">
@@ -7790,7 +7790,7 @@
       <c r="B57" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>516</v>
       </c>
       <c r="D57" s="2">
@@ -7804,7 +7804,7 @@
       <c r="B58" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>518</v>
       </c>
       <c r="D58" s="2">
@@ -7818,7 +7818,7 @@
       <c r="B59" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>520</v>
       </c>
       <c r="D59" s="2">
@@ -7832,7 +7832,7 @@
       <c r="B60" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>522</v>
       </c>
       <c r="D60" s="2">
@@ -7846,7 +7846,7 @@
       <c r="B61" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>524</v>
       </c>
       <c r="D61" s="2">
@@ -7860,7 +7860,7 @@
       <c r="B62" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>526</v>
       </c>
       <c r="D62" s="2">

</xml_diff>